<commit_message>
before all annotations geändert, lvtestfall gelöscht da keine testerwartung eingetragen
</commit_message>
<xml_diff>
--- a/src/test/resources/lv-projekte.xlsx
+++ b/src/test/resources/lv-projekte.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17030"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ProjektPortfolio\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="14730" windowHeight="2610" tabRatio="429"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="51">
   <si>
     <t>month</t>
   </si>
@@ -174,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -217,6 +222,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -493,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD39" sqref="AD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1356,8 +1364,8 @@
       <c r="J39" s="1">
         <v>42705</v>
       </c>
-      <c r="K39" t="s">
-        <v>13</v>
+      <c r="K39" s="1">
+        <v>42705</v>
       </c>
       <c r="L39" t="s">
         <v>13</v>
@@ -1374,8 +1382,8 @@
       <c r="P39" t="s">
         <v>13</v>
       </c>
-      <c r="Q39" t="s">
-        <v>13</v>
+      <c r="Q39" s="1">
+        <v>42705</v>
       </c>
       <c r="R39" s="1">
         <v>42614</v>

</xml_diff>